<commit_message>
finished IRR and consensus sheet. Next step Cohen's k and final sheet with 1 row per paper.
</commit_message>
<xml_diff>
--- a/Procedure Process Record.xlsx
+++ b/Procedure Process Record.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Step</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>S17</t>
+  </si>
+  <si>
+    <t>Final feature extraction consensus sheet</t>
+  </si>
+  <si>
+    <t>S18</t>
   </si>
 </sst>
 </file>
@@ -1045,6 +1051,26 @@
         <v>42</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="C26" s="8">
+        <v>45236.0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>73.0</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2"/>

</xml_diff>